<commit_message>
création classe Sprite avec les commentaires nécessaires, à peaufiner. Doit créer les formes dérivées et la version serializable
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456BEE61-08D0-4B5D-9082-C773BF590A1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F5CF4-705A-418D-AAA6-7BC7B8B326A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Jour</t>
   </si>
@@ -80,37 +80,10 @@
     <t>Planification</t>
   </si>
   <si>
-    <t>Total 08.mai</t>
-  </si>
-  <si>
-    <t>Total 09.mai</t>
-  </si>
-  <si>
     <t>Temps</t>
   </si>
   <si>
-    <t>Total 14.mai</t>
-  </si>
-  <si>
-    <t>Total 15.mai</t>
-  </si>
-  <si>
-    <t>Total 16.mai</t>
-  </si>
-  <si>
-    <t>Total 20.mai</t>
-  </si>
-  <si>
-    <t>Total 22.mai</t>
-  </si>
-  <si>
-    <t>Total 23.mai</t>
-  </si>
-  <si>
     <t>Lecture détaillée du cahier des charges</t>
-  </si>
-  <si>
-    <t>Le planning a été donné par les experts dans l'énoncé et M. Bonvin me l'a fourni et version .xlsx. Analyse calme du planning.</t>
   </si>
   <si>
     <t>Lecture détaillé de l'énoncé et réflexion sur les différents points.</t>
@@ -185,6 +158,42 @@
       </rPr>
       <t xml:space="preserve"> panels de propriétés.</t>
     </r>
+  </si>
+  <si>
+    <t>Décidé de ne pas faire une classe "Calque" --&gt; peu pertinent</t>
+  </si>
+  <si>
+    <t>Bilan</t>
+  </si>
+  <si>
+    <t>Globalement bien, perdu un peu de temps avec la documentation au départ.</t>
+  </si>
+  <si>
+    <t>à peaufiner / méthodes à revoir plus tard</t>
+  </si>
+  <si>
+    <t>Création de la classe sprite</t>
+  </si>
+  <si>
+    <t>Le planning a été donné dans l'énoncé et M. Bonvin me l'a fourni et version .xlsx. Analyse calme du planning.</t>
+  </si>
+  <si>
+    <t>Total 26.mai</t>
+  </si>
+  <si>
+    <t>Total 27.mai</t>
+  </si>
+  <si>
+    <t>Total 28.mai</t>
+  </si>
+  <si>
+    <t>Total 1.juin</t>
+  </si>
+  <si>
+    <t>Total 2.juin</t>
+  </si>
+  <si>
+    <t>Total 3.juin</t>
   </si>
 </sst>
 </file>
@@ -525,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -686,6 +695,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -726,8 +741,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D62" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D62" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D51" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -1227,7 +1242,7 @@
     </row>
     <row r="7" spans="2:26" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="20"/>
@@ -1254,7 +1269,7 @@
     </row>
     <row r="8" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="20"/>
@@ -1281,7 +1296,7 @@
     </row>
     <row r="9" spans="2:26" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="14" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="18"/>
@@ -1308,7 +1323,7 @@
     </row>
     <row r="10" spans="2:26" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
@@ -1519,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1655,7 +1670,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="51"/>
-      <c r="D4" s="38"/>
+      <c r="D4" s="55"/>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
@@ -1706,7 +1721,7 @@
     </row>
     <row r="6" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C6" s="43"/>
       <c r="D6" s="50"/>
@@ -1733,7 +1748,7 @@
     </row>
     <row r="7" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C7" s="43"/>
       <c r="D7" s="44"/>
@@ -1760,7 +1775,7 @@
     </row>
     <row r="8" spans="2:28" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="14" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
@@ -1787,7 +1802,7 @@
     </row>
     <row r="9" spans="2:28" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="15" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C9" s="43"/>
       <c r="D9" s="44"/>
@@ -1872,7 +1887,7 @@
       </c>
       <c r="C12" s="52"/>
       <c r="D12" s="47"/>
-      <c r="E12" s="41"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="41"/>
       <c r="G12" s="41"/>
       <c r="H12" s="41"/>
@@ -1953,7 +1968,7 @@
       </c>
       <c r="C15" s="48"/>
       <c r="D15" s="49"/>
-      <c r="E15" s="45"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="45"/>
       <c r="G15" s="45"/>
       <c r="H15" s="45"/>
@@ -1998,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K62"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2021,7 +2036,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>12</v>
@@ -2033,13 +2048,13 @@
         <v>43976</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C2" s="8">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2053,7 +2068,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2067,7 +2082,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2075,13 +2090,13 @@
         <v>43976</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C5" s="9">
         <v>6.25E-2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2089,10 +2104,13 @@
         <v>43976</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C6" s="9">
         <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2100,7 +2118,7 @@
         <v>43976</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C7" s="9">
         <v>1.3888888888888888E-2</v>
@@ -2117,7 +2135,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2125,13 +2143,13 @@
         <v>43976</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C9" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2139,50 +2157,68 @@
         <v>43976</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C10" s="9">
         <v>6.25E-2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="B11" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C11" s="11">
         <f>SUM(C2:C10)</f>
         <v>0.33333333333333331</v>
       </c>
+      <c r="D11" s="10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>43977</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C12" s="9">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>43977</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="8">
+        <v>8.3333333333333329E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>43977</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="8">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
@@ -2198,11 +2234,11 @@
     </row>
     <row r="17" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C17" s="11">
         <f>SUM(C12:C16)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0.20833333333333331</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
@@ -2237,7 +2273,7 @@
     </row>
     <row r="23" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="10" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C23" s="11">
         <f>SUM(C18:C22)</f>
@@ -2246,247 +2282,156 @@
     </row>
     <row r="24" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
-        <v>43598</v>
+        <v>43979</v>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
-        <v>43598</v>
+        <v>43979</v>
       </c>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
-        <v>43598</v>
+        <v>43979</v>
       </c>
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
-        <v>43598</v>
+        <v>43979</v>
       </c>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
-        <v>43598</v>
-      </c>
-      <c r="C28" s="4"/>
+    <row r="28" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="11">
+        <f>SUM(C26:C27)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
-        <v>43598</v>
+        <v>43983</v>
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
-        <v>43599</v>
-      </c>
-      <c r="C31" s="4"/>
+    <row r="30" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>43983</v>
+      </c>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="11">
+        <f>SUM(C29:C30)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
-        <v>43599</v>
+        <v>43984</v>
       </c>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
-        <v>43599</v>
+        <v>43984</v>
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C34" s="11">
-        <f>SUM(C31:C33)</f>
+        <f>SUM(C32:C33)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
-        <v>43600</v>
+        <v>43985</v>
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
-        <v>43600</v>
+        <v>43985</v>
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="10" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C37" s="11">
         <f>SUM(C35:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
-        <v>43601</v>
-      </c>
+    <row r="38" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7">
-        <v>43601</v>
-      </c>
+    <row r="39" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="11">
-        <f>SUM(C38:C39)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7">
-        <v>43605</v>
-      </c>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7">
-        <v>43605</v>
-      </c>
+    <row r="40" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7">
-        <v>43605</v>
-      </c>
+    <row r="43" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7">
-        <v>43605</v>
-      </c>
+    <row r="44" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
-        <v>43605</v>
-      </c>
+    <row r="45" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7">
-        <v>43605</v>
-      </c>
+    <row r="46" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="3"/>
       <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7">
-        <v>43605</v>
-      </c>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C48" s="11">
-        <f>SUM(C41:C47)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7">
-        <v>43606</v>
-      </c>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7"/>
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="11"/>
-    </row>
-    <row r="53" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="7">
-        <v>43607</v>
-      </c>
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="7">
-        <v>43607</v>
-      </c>
-      <c r="C54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="7">
-        <v>43607</v>
-      </c>
-      <c r="C55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="7">
-        <v>43607</v>
-      </c>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="7">
-        <v>43607</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C58" s="11">
-        <f>SUM(C53:C57)</f>
-        <v>0</v>
-      </c>
-      <c r="D58" s="10"/>
-    </row>
-    <row r="59" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="7">
-        <v>43608</v>
-      </c>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="7">
-        <v>43608</v>
-      </c>
-      <c r="C60" s="4"/>
-    </row>
-    <row r="61" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="7">
-        <v>43608</v>
-      </c>
-      <c r="C61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C62" s="11">
-        <f>SUM(C59:C61)</f>
-        <v>0</v>
-      </c>
+    <row r="51" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout des classes Rond et Carre, rien de fonctionnel pour le moment
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F5CF4-705A-418D-AAA6-7BC7B8B326A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABBE213-105D-4E92-8849-5ED02D3BA8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Jour</t>
   </si>
@@ -160,18 +160,12 @@
     </r>
   </si>
   <si>
-    <t>Décidé de ne pas faire une classe "Calque" --&gt; peu pertinent</t>
-  </si>
-  <si>
     <t>Bilan</t>
   </si>
   <si>
     <t>Globalement bien, perdu un peu de temps avec la documentation au départ.</t>
   </si>
   <si>
-    <t>à peaufiner / méthodes à revoir plus tard</t>
-  </si>
-  <si>
     <t>Création de la classe sprite</t>
   </si>
   <si>
@@ -194,6 +188,30 @@
   </si>
   <si>
     <t>Total 3.juin</t>
+  </si>
+  <si>
+    <t>Création de formes simples</t>
+  </si>
+  <si>
+    <t>Classes : Carre.cs, Rond.cs</t>
+  </si>
+  <si>
+    <t>Mise à jour visual studio</t>
+  </si>
+  <si>
+    <t>Entretien avec M. Bonvin</t>
+  </si>
+  <si>
+    <t>Juste voir si tout allait bien, discussion globale</t>
+  </si>
+  <si>
+    <t>Décidé de ne pas faire une classe "Calque" --&gt; peu pertinent. Diagramme pas tout à fait terminé</t>
+  </si>
+  <si>
+    <t>Terminé. Une conversion devra être faite du Sprite (qui hérite de Picturebox) à SpriteSerializable (qui sert surtout à contenir les propriétés des sprites).</t>
+  </si>
+  <si>
+    <t>Manque des choses, réflexion nécessaire</t>
   </si>
 </sst>
 </file>
@@ -690,17 +708,17 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -741,8 +759,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D51" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D53" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -1068,50 +1086,50 @@
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="55">
         <v>1</v>
       </c>
-      <c r="D3" s="54"/>
-      <c r="E3" s="53">
+      <c r="D3" s="56"/>
+      <c r="E3" s="55">
         <v>2</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="53">
+      <c r="F3" s="56"/>
+      <c r="G3" s="55">
         <v>3</v>
       </c>
-      <c r="H3" s="54"/>
-      <c r="I3" s="53">
+      <c r="H3" s="56"/>
+      <c r="I3" s="55">
         <v>4</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="53">
+      <c r="J3" s="56"/>
+      <c r="K3" s="55">
         <v>5</v>
       </c>
-      <c r="L3" s="54"/>
-      <c r="M3" s="53">
+      <c r="L3" s="56"/>
+      <c r="M3" s="55">
         <v>6</v>
       </c>
-      <c r="N3" s="54"/>
-      <c r="O3" s="53">
+      <c r="N3" s="56"/>
+      <c r="O3" s="55">
         <v>7</v>
       </c>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="53">
+      <c r="P3" s="56"/>
+      <c r="Q3" s="55">
         <v>8</v>
       </c>
-      <c r="R3" s="54"/>
-      <c r="S3" s="53">
+      <c r="R3" s="56"/>
+      <c r="S3" s="55">
         <v>9</v>
       </c>
-      <c r="T3" s="54"/>
-      <c r="U3" s="53">
+      <c r="T3" s="56"/>
+      <c r="U3" s="55">
         <v>10</v>
       </c>
-      <c r="V3" s="54"/>
-      <c r="W3" s="53">
+      <c r="V3" s="56"/>
+      <c r="W3" s="55">
         <v>11</v>
       </c>
-      <c r="X3" s="54"/>
+      <c r="X3" s="56"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
@@ -1535,7 +1553,7 @@
   <dimension ref="B1:AB16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1549,50 +1567,50 @@
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="53">
+      <c r="C2" s="55">
         <v>1</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="53">
+      <c r="D2" s="56"/>
+      <c r="E2" s="55">
         <v>2</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="53">
+      <c r="F2" s="56"/>
+      <c r="G2" s="55">
         <v>3</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="53">
+      <c r="H2" s="56"/>
+      <c r="I2" s="55">
         <v>4</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="53">
+      <c r="J2" s="56"/>
+      <c r="K2" s="55">
         <v>5</v>
       </c>
-      <c r="L2" s="54"/>
-      <c r="M2" s="53">
+      <c r="L2" s="56"/>
+      <c r="M2" s="55">
         <v>6</v>
       </c>
-      <c r="N2" s="54"/>
-      <c r="O2" s="53">
+      <c r="N2" s="56"/>
+      <c r="O2" s="55">
         <v>7</v>
       </c>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="53">
+      <c r="P2" s="56"/>
+      <c r="Q2" s="55">
         <v>8</v>
       </c>
-      <c r="R2" s="54"/>
-      <c r="S2" s="53">
+      <c r="R2" s="56"/>
+      <c r="S2" s="55">
         <v>9</v>
       </c>
-      <c r="T2" s="54"/>
-      <c r="U2" s="53">
+      <c r="T2" s="56"/>
+      <c r="U2" s="55">
         <v>10</v>
       </c>
-      <c r="V2" s="54"/>
-      <c r="W2" s="53">
+      <c r="V2" s="56"/>
+      <c r="W2" s="55">
         <v>11</v>
       </c>
-      <c r="X2" s="54"/>
+      <c r="X2" s="56"/>
     </row>
     <row r="3" spans="2:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
@@ -1670,7 +1688,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="51"/>
-      <c r="D4" s="55"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
@@ -1696,7 +1714,7 @@
       <c r="B5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="40"/>
+      <c r="C5" s="52"/>
       <c r="D5" s="41"/>
       <c r="E5" s="41"/>
       <c r="F5" s="41"/>
@@ -1753,7 +1771,7 @@
       <c r="C7" s="43"/>
       <c r="D7" s="44"/>
       <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="F7" s="47"/>
       <c r="G7" s="41"/>
       <c r="H7" s="41"/>
       <c r="I7" s="41"/>
@@ -1780,7 +1798,7 @@
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="F8" s="47"/>
       <c r="G8" s="41"/>
       <c r="H8" s="41"/>
       <c r="I8" s="41"/>
@@ -1888,7 +1906,7 @@
       <c r="C12" s="52"/>
       <c r="D12" s="47"/>
       <c r="E12" s="47"/>
-      <c r="F12" s="41"/>
+      <c r="F12" s="47"/>
       <c r="G12" s="41"/>
       <c r="H12" s="41"/>
       <c r="I12" s="41"/>
@@ -1968,8 +1986,8 @@
       </c>
       <c r="C15" s="48"/>
       <c r="D15" s="49"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="45"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
       <c r="G15" s="45"/>
       <c r="H15" s="45"/>
       <c r="I15" s="45"/>
@@ -1994,17 +2012,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2013,10 +2031,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2082,7 +2100,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2104,13 +2122,10 @@
         <v>43976</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C6" s="9">
-        <v>2.7777777777777776E-2</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2121,7 +2136,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="9">
-        <v>1.3888888888888888E-2</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2157,42 +2172,42 @@
         <v>43976</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>43976</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C11" s="9">
         <v>6.25E-2</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+    <row r="12" spans="1:11" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="11">
+        <f>SUM(C2:C11)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="11">
-        <f>SUM(C2:C10)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
-        <v>43977</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="9">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2200,202 +2215,236 @@
         <v>43977</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="8">
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>43977</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C13" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
       <c r="B14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="8">
-        <v>8.3333333333333329E-2</v>
+        <v>31</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>43977</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.10416666666666667</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>43977</v>
       </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="11">
-        <f>SUM(C12:C16)</f>
-        <v>0.20833333333333331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>43977</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="8">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
-        <v>43978</v>
-      </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <v>43978</v>
-      </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>43977</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="9">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="11">
+        <f>SUM(C13:C18)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>43978</v>
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>43978</v>
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>43978</v>
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="11">
-        <f>SUM(C18:C22)</f>
+    <row r="23" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>43978</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>43978</v>
+      </c>
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="11">
+        <f>SUM(C20:C24)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>43979</v>
-      </c>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7">
-        <v>43979</v>
-      </c>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>43979</v>
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>43979</v>
       </c>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="11">
-        <f>SUM(C26:C27)</f>
+    <row r="28" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>43979</v>
+      </c>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>43979</v>
+      </c>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="11">
+        <f>SUM(C28:C29)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
+    <row r="31" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
         <v>43983</v>
       </c>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
         <v>43983</v>
       </c>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="11">
-        <f>SUM(C29:C30)</f>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="11">
+        <f>SUM(C31:C32)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
+    <row r="34" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
         <v>43984</v>
       </c>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
-        <v>43984</v>
-      </c>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="11">
-        <f>SUM(C32:C33)</f>
-        <v>0</v>
-      </c>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
+        <v>43984</v>
+      </c>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="11">
+        <f>SUM(C34:C35)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
         <v>43985</v>
       </c>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
         <v>43985</v>
       </c>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="11">
-        <f>SUM(C35:C36)</f>
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="11">
+        <f>SUM(C37:C38)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="4"/>
-    </row>
     <row r="40" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="11"/>
+    <row r="41" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="C43" s="4"/>
+    <row r="43" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="11"/>
     </row>
     <row r="44" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
@@ -2405,33 +2454,41 @@
       <c r="A45" s="7"/>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
-      <c r="B46" s="3"/>
       <c r="C46" s="4"/>
-      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
-      <c r="B47" s="10"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="10"/>
-    </row>
-    <row r="48" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
+      <c r="B48" s="3"/>
       <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:3" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="10"/>
+    </row>
+    <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
       <c r="C50" s="4"/>
     </row>
-    <row r="51" spans="1:3" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
+    <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7"/>
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="7"/>
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="11"/>
+      <c r="C53" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Création de sprites (basiques) fonctionnelle avec bug
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABBE213-105D-4E92-8849-5ED02D3BA8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4C3EB3-31C3-41AD-A0FB-1F8D7E65E3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>Jour</t>
   </si>
@@ -212,6 +212,24 @@
   </si>
   <si>
     <t>Manque des choses, réflexion nécessaire</t>
+  </si>
+  <si>
+    <t>Classe Logo et Sprites</t>
+  </si>
+  <si>
+    <t>Ajout des premières méthodes, marche</t>
+  </si>
+  <si>
+    <t>Création de classes de formes simples</t>
+  </si>
+  <si>
+    <t>Sur création des formes (ci-dessus)</t>
+  </si>
+  <si>
+    <t>Problème, L'appli plante dans certaines conditions (Si on ajoute 2 carrés de suite, etc) --&gt; pourquoi ? À corriger demain</t>
+  </si>
+  <si>
+    <t>Perdu pas mal de temps avec erreur quand on crée une forme, bien avancé la doc</t>
   </si>
 </sst>
 </file>
@@ -1552,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1772,8 +1790,8 @@
       <c r="D7" s="44"/>
       <c r="E7" s="41"/>
       <c r="F7" s="47"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
       <c r="I7" s="41"/>
       <c r="J7" s="41"/>
       <c r="K7" s="41"/>
@@ -1799,8 +1817,8 @@
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
       <c r="F8" s="47"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
       <c r="I8" s="41"/>
       <c r="J8" s="41"/>
       <c r="K8" s="41"/>
@@ -1881,7 +1899,7 @@
       <c r="E11" s="41"/>
       <c r="F11" s="41"/>
       <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
+      <c r="H11" s="47"/>
       <c r="I11" s="41"/>
       <c r="J11" s="41"/>
       <c r="K11" s="41"/>
@@ -1907,8 +1925,8 @@
       <c r="D12" s="47"/>
       <c r="E12" s="47"/>
       <c r="F12" s="47"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
       <c r="I12" s="41"/>
       <c r="J12" s="41"/>
       <c r="K12" s="41"/>
@@ -1988,8 +2006,8 @@
       <c r="D15" s="49"/>
       <c r="E15" s="54"/>
       <c r="F15" s="54"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="45"/>
       <c r="J15" s="45"/>
       <c r="K15" s="45"/>
@@ -2033,15 +2051,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="26.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" style="5"/>
+    <col min="3" max="3" width="15.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.77734375" style="3"/>
   </cols>
@@ -2266,7 +2284,7 @@
         <v>43977</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C17" s="8">
         <v>2.0833333333333332E-2</v>
@@ -2290,6 +2308,9 @@
       </c>
     </row>
     <row r="19" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="B19" s="10" t="s">
         <v>38</v>
       </c>
@@ -2298,43 +2319,83 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>43978</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="B20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="8">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>43978</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.11805555555555557</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>43978</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="B22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>43978</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>43978</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
     </row>
     <row r="25" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="B25" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="11">
         <f>SUM(C20:C24)</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Tout marche (ajout + modif des sprites), ajout triangle, manque texte
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4C3EB3-31C3-41AD-A0FB-1F8D7E65E3C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A00C7C5-9CD2-4B08-90D4-2060610A51DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <t>Jour</t>
   </si>
@@ -230,6 +230,30 @@
   </si>
   <si>
     <t>Perdu pas mal de temps avec erreur quand on crée une forme, bien avancé la doc</t>
+  </si>
+  <si>
+    <t>Erreur corrigée</t>
+  </si>
+  <si>
+    <t>Modification et affichage des bonnes propriétés</t>
+  </si>
+  <si>
+    <t>Tout fonctionne</t>
+  </si>
+  <si>
+    <t>Création de la classe Triangle.cs</t>
+  </si>
+  <si>
+    <t>Bonne journée, rien à redire.</t>
+  </si>
+  <si>
+    <t>Revue du code</t>
+  </si>
+  <si>
+    <t>Modification de certaines choses (ajout de méthodes pour faire plus propres, etc) + commentaires détaillés</t>
+  </si>
+  <si>
+    <t>Bien avancé le prorgamme et pas perdu de temps aujourd'hui (aurait pu avancer un peu plus la doc). Il faut rajouter le texte maintenant.</t>
   </si>
 </sst>
 </file>
@@ -777,8 +801,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D53" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D54" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -1089,7 +1113,7 @@
   <dimension ref="B2:Z17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1571,7 +1595,7 @@
   <dimension ref="B1:AB16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1819,8 +1843,8 @@
       <c r="F8" s="47"/>
       <c r="G8" s="47"/>
       <c r="H8" s="47"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
       <c r="K8" s="41"/>
       <c r="L8" s="41"/>
       <c r="M8" s="41"/>
@@ -1927,8 +1951,8 @@
       <c r="F12" s="47"/>
       <c r="G12" s="47"/>
       <c r="H12" s="47"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
       <c r="K12" s="41"/>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
@@ -2008,8 +2032,8 @@
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
       <c r="H15" s="54"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="54"/>
       <c r="K15" s="45"/>
       <c r="L15" s="45"/>
       <c r="M15" s="45"/>
@@ -2049,10 +2073,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A25" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2318,6 +2342,9 @@
         <f>SUM(C13:C18)</f>
         <v>0.33333333333333331</v>
       </c>
+      <c r="D19" s="10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
@@ -2402,40 +2429,83 @@
       <c r="A26" s="7">
         <v>43979</v>
       </c>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>43979</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="B27" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <v>43979</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="B28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="8">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>43979</v>
       </c>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="10" t="s">
+      <c r="B29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="9">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>43979</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="8">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="11">
-        <f>SUM(C28:C29)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
-        <v>43983</v>
-      </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="11">
+        <f>SUM(C26:C30)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
@@ -2444,19 +2514,23 @@
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="10" t="s">
+      <c r="A33" s="7">
+        <v>43983</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="11">
-        <f>SUM(C31:C32)</f>
+      <c r="C34" s="11">
+        <f>SUM(C32:C33)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
-        <v>43984</v>
-      </c>
-      <c r="C34" s="4"/>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
@@ -2465,19 +2539,23 @@
       <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="10" t="s">
+      <c r="A36" s="7">
+        <v>43984</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="11">
-        <f>SUM(C34:C35)</f>
+      <c r="C37" s="11">
+        <f>SUM(C35:C36)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7">
-        <v>43985</v>
-      </c>
-      <c r="C37" s="4"/>
+      <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
@@ -2486,30 +2564,38 @@
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="10" t="s">
+      <c r="A39" s="7">
+        <v>43985</v>
+      </c>
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="11">
-        <f>SUM(C37:C38)</f>
+      <c r="C40" s="11">
+        <f>SUM(C38:C39)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="C40" s="4"/>
-    </row>
     <row r="41" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
       <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="11"/>
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="10"/>
     </row>
     <row r="45" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
@@ -2530,14 +2616,14 @@
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="10"/>
+      <c r="A49" s="7"/>
+      <c r="C49" s="4"/>
     </row>
     <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
-      <c r="C50" s="4"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7"/>
@@ -2548,8 +2634,16 @@
       <c r="C52" s="4"/>
     </row>
     <row r="53" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
+      <c r="A53" s="7"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajoute de la classe texte, fonctionne mais manque la modif
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A00C7C5-9CD2-4B08-90D4-2060610A51DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5824384-9775-47C1-84EC-4F3D6D88D98B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>Jour</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Total 1.juin</t>
   </si>
   <si>
-    <t>Total 2.juin</t>
-  </si>
-  <si>
     <t>Total 3.juin</t>
   </si>
   <si>
@@ -254,6 +251,22 @@
   </si>
   <si>
     <t>Bien avancé le prorgamme et pas perdu de temps aujourd'hui (aurait pu avancer un peu plus la doc). Il faut rajouter le texte maintenant.</t>
+  </si>
+  <si>
+    <t>Total 29.mai</t>
+  </si>
+  <si>
+    <t>Sur conseil de M. Bonvin, j'ai passé un moment à améliorer la documentation et à la détailler.</t>
+  </si>
+  <si>
+    <t>M. Bonvin a voulu s'assurer qu'on partait dans la bonne direction.
+Bilan : Partie technique est bien avancée, aucun commentaire la dessus. La doc est insuffisante, trop breve,  à améliorer.</t>
+  </si>
+  <si>
+    <t>Création classe Texte</t>
+  </si>
+  <si>
+    <t>Fonctionne correctement, affichage aussi. Plus qu'à ajouter la modification</t>
   </si>
 </sst>
 </file>
@@ -801,8 +814,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D54" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D55" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -1594,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1924,8 +1937,8 @@
       <c r="F11" s="41"/>
       <c r="G11" s="41"/>
       <c r="H11" s="47"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
       <c r="K11" s="41"/>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
@@ -1953,7 +1966,7 @@
       <c r="H12" s="47"/>
       <c r="I12" s="47"/>
       <c r="J12" s="47"/>
-      <c r="K12" s="41"/>
+      <c r="K12" s="47"/>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
       <c r="N12" s="41"/>
@@ -2034,7 +2047,7 @@
       <c r="H15" s="54"/>
       <c r="I15" s="54"/>
       <c r="J15" s="54"/>
-      <c r="K15" s="45"/>
+      <c r="K15" s="54"/>
       <c r="L15" s="45"/>
       <c r="M15" s="45"/>
       <c r="N15" s="45"/>
@@ -2054,17 +2067,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2073,10 +2086,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2164,7 +2177,7 @@
         <v>43976</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="9">
         <v>6.9444444444444441E-3</v>
@@ -2220,7 +2233,7 @@
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2275,7 +2288,7 @@
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2300,7 +2313,7 @@
         <v>0.14583333333333334</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2308,13 +2321,13 @@
         <v>43977</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="8">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2322,13 +2335,13 @@
         <v>43977</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="9">
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2343,7 +2356,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2351,13 +2364,13 @@
         <v>43978</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="8">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2376,13 +2389,13 @@
         <v>43978</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="8">
         <v>0.10416666666666667</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2396,7 +2409,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2404,7 +2417,7 @@
         <v>43978</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="8">
         <v>6.9444444444444441E-3</v>
@@ -2422,7 +2435,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2430,13 +2443,13 @@
         <v>43979</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="8">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2444,13 +2457,13 @@
         <v>43979</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="8">
         <v>0.14583333333333334</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2458,13 +2471,13 @@
         <v>43979</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="8">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2472,13 +2485,13 @@
         <v>43979</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="9">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2504,64 +2517,86 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D31" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>43980</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="9">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>43980</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.125</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>43980</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0.125</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
+      <c r="C35" s="11">
+        <f>SUM(C32:C34)</f>
+        <v>0.26041666666666663</v>
+      </c>
+      <c r="D35" s="10"/>
+    </row>
+    <row r="36" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
         <v>43983</v>
       </c>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
         <v>43983</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C34" s="11">
-        <f>SUM(C32:C33)</f>
+      <c r="C38" s="11">
+        <f>SUM(C36:C37)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="10"/>
-    </row>
-    <row r="35" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
-        <v>43984</v>
-      </c>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
-        <v>43984</v>
-      </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="11">
-        <f>SUM(C35:C36)</f>
-        <v>0</v>
-      </c>
-      <c r="D37" s="10"/>
-    </row>
-    <row r="38" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
-        <v>43985</v>
-      </c>
-      <c r="C38" s="4"/>
+      <c r="D38" s="10"/>
     </row>
     <row r="39" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
@@ -2570,36 +2605,38 @@
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="11">
-        <f>SUM(C38:C39)</f>
+      <c r="A40" s="7">
+        <v>43985</v>
+      </c>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="11">
+        <f>SUM(C39:C40)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="C41" s="4"/>
-    </row>
     <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
+    <row r="43" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="4"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="10"/>
+    </row>
+    <row r="44" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
@@ -2609,41 +2646,45 @@
       <c r="A47" s="7"/>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
-      <c r="B48" s="3"/>
       <c r="C48" s="4"/>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
+      <c r="B49" s="3"/>
       <c r="C49" s="4"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="10"/>
+      <c r="A50" s="7"/>
+      <c r="C50" s="4"/>
     </row>
     <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="C51" s="4"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7"/>
-      <c r="B53" s="3"/>
       <c r="C53" s="4"/>
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="10"/>
+    </row>
+    <row r="54" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout polygone et la modif du texte fonctionne
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5824384-9775-47C1-84EC-4F3D6D88D98B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD4B890-4E16-4A5C-96CF-98D92A41A3CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
   <si>
     <t>Jour</t>
   </si>
@@ -181,7 +181,7 @@
     <t>Total 28.mai</t>
   </si>
   <si>
-    <t>Total 1.juin</t>
+    <t>Total 2.juin</t>
   </si>
   <si>
     <t>Total 3.juin</t>
@@ -266,7 +266,28 @@
     <t>Création classe Texte</t>
   </si>
   <si>
-    <t>Fonctionne correctement, affichage aussi. Plus qu'à ajouter la modification</t>
+    <t>Modification et affichage des bonnes propriétés du texte</t>
+  </si>
+  <si>
+    <t>Fonctionne</t>
+  </si>
+  <si>
+    <t>Fonctionne correctement, affichage aussi. Plus qu'à ajouter la modification.</t>
+  </si>
+  <si>
+    <t>Total 4.juin</t>
+  </si>
+  <si>
+    <t>Création de polygone</t>
+  </si>
+  <si>
+    <t>Transparence d'un calque</t>
+  </si>
+  <si>
+    <t>bien avancé mais je dois plus attention à être plus régulier avec la doc que je produit.</t>
+  </si>
+  <si>
+    <t>Début d'export d'image</t>
   </si>
 </sst>
 </file>
@@ -607,7 +628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -773,6 +794,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -814,8 +838,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D55" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D58" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D58" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -1126,7 +1150,7 @@
   <dimension ref="B2:Z17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+      <selection activeCell="AC15" sqref="AC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1607,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1858,8 +1882,8 @@
       <c r="H8" s="47"/>
       <c r="I8" s="47"/>
       <c r="J8" s="47"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
       <c r="M8" s="41"/>
       <c r="N8" s="41"/>
       <c r="O8" s="41"/>
@@ -1887,8 +1911,8 @@
       <c r="J9" s="41"/>
       <c r="K9" s="41"/>
       <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
       <c r="O9" s="41"/>
       <c r="P9" s="41"/>
       <c r="Q9" s="41"/>
@@ -1939,10 +1963,10 @@
       <c r="H11" s="47"/>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
       <c r="O11" s="41"/>
       <c r="P11" s="41"/>
       <c r="Q11" s="41"/>
@@ -1967,9 +1991,9 @@
       <c r="I12" s="47"/>
       <c r="J12" s="47"/>
       <c r="K12" s="47"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
       <c r="O12" s="41"/>
       <c r="P12" s="41"/>
       <c r="Q12" s="41"/>
@@ -2048,9 +2072,9 @@
       <c r="I15" s="54"/>
       <c r="J15" s="54"/>
       <c r="K15" s="54"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="54"/>
       <c r="O15" s="45"/>
       <c r="P15" s="45"/>
       <c r="Q15" s="45"/>
@@ -2086,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A33" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2559,132 +2583,191 @@
         <v>0.125</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>43980</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10" t="s">
+      <c r="C35" s="8">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="11">
-        <f>SUM(C32:C34)</f>
-        <v>0.26041666666666663</v>
-      </c>
-      <c r="D35" s="10"/>
-    </row>
-    <row r="36" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
-        <v>43983</v>
-      </c>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="11">
+        <f>SUM(C32:C35)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
-        <v>43983</v>
-      </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
+        <v>43984</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="8">
+        <v>8.3333333333333329E-2</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10" t="s">
+      <c r="A38" s="7">
+        <v>43984</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="8">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>43984</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="8">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="57"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="11">
-        <f>SUM(C36:C37)</f>
+      <c r="C41" s="11">
+        <f>SUM(C37:C40)</f>
+        <v>0.20833333333333331</v>
+      </c>
+      <c r="D41" s="10"/>
+    </row>
+    <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>43985</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
+        <v>43985</v>
+      </c>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" s="11">
+        <f>SUM(C42:C43)</f>
         <v>0</v>
       </c>
-      <c r="D38" s="10"/>
-    </row>
-    <row r="39" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7">
-        <v>43985</v>
-      </c>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7">
-        <v>43985</v>
-      </c>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="11">
-        <f>SUM(C39:C40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="10"/>
+      <c r="A45" s="7">
+        <v>43986</v>
+      </c>
+      <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
+      <c r="A46" s="7">
+        <v>43986</v>
+      </c>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
+    <row r="47" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>72</v>
+      </c>
       <c r="C47" s="4"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="10"/>
+    </row>
+    <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
-      <c r="B49" s="3"/>
       <c r="C49" s="4"/>
-      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
       <c r="C50" s="4"/>
     </row>
     <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7"/>
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
+      <c r="B52" s="3"/>
       <c r="C52" s="4"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7"/>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="7"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="3"/>
+    <row r="54" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="10"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="10"/>
+      <c r="A55" s="7"/>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="7"/>
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sérialisation + désérialisation fonctionne. Manques quelques détails à finaliser
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065D68EE-5343-49F4-B124-F7E600BB8C97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35A24E1-C557-4A28-AB35-ADCD23DE8EA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
   <si>
     <t>Jour</t>
   </si>
@@ -291,6 +291,24 @@
   </si>
   <si>
     <t>Marche, réflexion nécessaire.</t>
+  </si>
+  <si>
+    <t>Correct au niveau de la documentation, encore à améliorer. Pas mal au niveau du code, bien avancé. Demain -&gt; serialisation</t>
+  </si>
+  <si>
+    <t>Conclusion -&gt; doc manque d'images</t>
+  </si>
+  <si>
+    <t>Enregistrement de logo (serialisation)</t>
+  </si>
+  <si>
+    <t>Perdu du temps avec une erreur.</t>
+  </si>
+  <si>
+    <t>Chargement d'un fichier (désérialisation)</t>
+  </si>
+  <si>
+    <t>Globalement bien avancé. Tous les 7 points sont presque tous remplis. Manque quelques finalisation</t>
   </si>
 </sst>
 </file>
@@ -838,8 +856,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D58" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D58" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D60" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D60" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -1631,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1913,8 +1931,8 @@
       <c r="L9" s="41"/>
       <c r="M9" s="41"/>
       <c r="N9" s="47"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
       <c r="Q9" s="41"/>
       <c r="R9" s="41"/>
       <c r="S9" s="41"/>
@@ -1967,8 +1985,8 @@
       <c r="L11" s="47"/>
       <c r="M11" s="47"/>
       <c r="N11" s="47"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
       <c r="Q11" s="41"/>
       <c r="R11" s="41"/>
       <c r="S11" s="41"/>
@@ -1994,8 +2012,8 @@
       <c r="L12" s="47"/>
       <c r="M12" s="47"/>
       <c r="N12" s="47"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
       <c r="Q12" s="41"/>
       <c r="R12" s="41"/>
       <c r="S12" s="41"/>
@@ -2075,8 +2093,8 @@
       <c r="L15" s="54"/>
       <c r="M15" s="54"/>
       <c r="N15" s="54"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
+      <c r="O15" s="54"/>
+      <c r="P15" s="54"/>
       <c r="Q15" s="45"/>
       <c r="R15" s="45"/>
       <c r="S15" s="45"/>
@@ -2110,10 +2128,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A41" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2645,7 +2663,7 @@
         <v>74</v>
       </c>
       <c r="C39" s="8">
-        <v>4.1666666666666664E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
       <c r="D39" s="3"/>
     </row>
@@ -2654,126 +2672,170 @@
         <v>43984</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>43984</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C41" s="8">
         <v>0.125</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10" t="s">
+    <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B42" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="11">
-        <f>SUM(C37:C40)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D41" s="10"/>
-    </row>
-    <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7">
-        <v>43985</v>
+      <c r="C42" s="11">
+        <f>SUM(C37:C41)</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>43985</v>
       </c>
-      <c r="C43" s="4"/>
+      <c r="B43" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="8">
+        <v>0.125</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="11">
-        <f>SUM(C42:C43)</f>
-        <v>0</v>
+      <c r="A44" s="7">
+        <v>43985</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="8">
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
+        <v>43985</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="8">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" s="11">
+        <f>SUM(C43:C45)</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
         <v>43986</v>
       </c>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7">
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7">
         <v>43986</v>
       </c>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="10" t="s">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B49" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
       <c r="C49" s="4"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
-      <c r="C50" s="4"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7"/>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
-      <c r="B52" s="3"/>
       <c r="C52" s="4"/>
-      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7"/>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="10"/>
+    <row r="54" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
       <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="10"/>
+    </row>
+    <row r="57" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
-      <c r="B57" s="3"/>
       <c r="C57" s="4"/>
-      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="10"/>
+      <c r="A58" s="7"/>
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrections mineures. Il manque quelques messages et sécurité (au niveau des fichiers).
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35A24E1-C557-4A28-AB35-ADCD23DE8EA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E41A049-5A4F-450B-B580-6025BBCC1CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
   <si>
     <t>Jour</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>Globalement bien avancé. Tous les 7 points sont presque tous remplis. Manque quelques finalisation</t>
+  </si>
+  <si>
+    <t>Corrections mineures</t>
   </si>
 </sst>
 </file>
@@ -856,8 +859,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D60" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D60" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D61" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D61" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -1649,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA12" sqref="AA12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q15" activeCellId="3" sqref="Q12 Q10 Q11 Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1960,7 +1963,7 @@
       <c r="N10" s="41"/>
       <c r="O10" s="41"/>
       <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
+      <c r="Q10" s="47"/>
       <c r="R10" s="41"/>
       <c r="S10" s="41"/>
       <c r="T10" s="41"/>
@@ -1987,7 +1990,7 @@
       <c r="N11" s="47"/>
       <c r="O11" s="47"/>
       <c r="P11" s="47"/>
-      <c r="Q11" s="41"/>
+      <c r="Q11" s="47"/>
       <c r="R11" s="41"/>
       <c r="S11" s="41"/>
       <c r="T11" s="41"/>
@@ -2014,7 +2017,7 @@
       <c r="N12" s="47"/>
       <c r="O12" s="47"/>
       <c r="P12" s="47"/>
-      <c r="Q12" s="41"/>
+      <c r="Q12" s="47"/>
       <c r="R12" s="41"/>
       <c r="S12" s="41"/>
       <c r="T12" s="41"/>
@@ -2095,7 +2098,7 @@
       <c r="N15" s="54"/>
       <c r="O15" s="54"/>
       <c r="P15" s="54"/>
-      <c r="Q15" s="45"/>
+      <c r="Q15" s="54"/>
       <c r="R15" s="45"/>
       <c r="S15" s="45"/>
       <c r="T15" s="45"/>
@@ -2128,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2765,33 +2768,53 @@
       <c r="A47" s="7">
         <v>43986</v>
       </c>
-      <c r="C47" s="4"/>
+      <c r="B47" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
     </row>
     <row r="48" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>43986</v>
       </c>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="10" t="s">
+      <c r="B48" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="8">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7">
+        <v>43986</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="8">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B50" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="10"/>
+      <c r="C50" s="11">
+        <f>SUM(C47:C49)</f>
+        <v>9.0277777777777762E-2</v>
+      </c>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="C51" s="4"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
@@ -2801,41 +2824,45 @@
       <c r="A53" s="7"/>
       <c r="C53" s="4"/>
     </row>
-    <row r="54" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
-      <c r="B54" s="3"/>
       <c r="C54" s="4"/>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
+      <c r="B55" s="3"/>
       <c r="C55" s="4"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="10"/>
-      <c r="B56" s="10"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="10"/>
+      <c r="A56" s="7"/>
+      <c r="C56" s="4"/>
     </row>
     <row r="57" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="7"/>
-      <c r="C57" s="4"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="10"/>
     </row>
     <row r="58" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7"/>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7"/>
-      <c r="B59" s="3"/>
       <c r="C59" s="4"/>
-      <c r="D59" s="3"/>
-    </row>
-    <row r="60" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="10"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="10"/>
+    </row>
+    <row r="60" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="7"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="10"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Surtout de la documentation...
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E41A049-5A4F-450B-B580-6025BBCC1CA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73140CBF-1685-4DFC-A220-FA1574EA50D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -1652,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q15" activeCellId="3" sqref="Q12 Q10 Q11 Q15"/>
     </sheetView>
   </sheetViews>
@@ -2133,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+    <sheetView topLeftCell="A41" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Juste remplis le planning effectif.
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73140CBF-1685-4DFC-A220-FA1574EA50D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0880AAD-05FA-429D-A02C-36972EB5644C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
   <si>
     <t>Jour</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>Corrections mineures</t>
+  </si>
+  <si>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>Entretien avec les experts</t>
+  </si>
+  <si>
+    <t>Avancement correct. Pas en retard mais le rythme pourrait être plus important au niveau de la doc.</t>
   </si>
 </sst>
 </file>
@@ -859,8 +868,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D61" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D61" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D63" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D63" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -1171,7 +1180,7 @@
   <dimension ref="B2:Z17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AB16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" activeCellId="3" sqref="Q12 Q10 Q11 Q15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1964,7 +1973,7 @@
       <c r="O10" s="41"/>
       <c r="P10" s="41"/>
       <c r="Q10" s="47"/>
-      <c r="R10" s="41"/>
+      <c r="R10" s="47"/>
       <c r="S10" s="41"/>
       <c r="T10" s="41"/>
       <c r="U10" s="41"/>
@@ -1991,7 +2000,7 @@
       <c r="O11" s="47"/>
       <c r="P11" s="47"/>
       <c r="Q11" s="47"/>
-      <c r="R11" s="41"/>
+      <c r="R11" s="47"/>
       <c r="S11" s="41"/>
       <c r="T11" s="41"/>
       <c r="U11" s="41"/>
@@ -2018,7 +2027,7 @@
       <c r="O12" s="47"/>
       <c r="P12" s="47"/>
       <c r="Q12" s="47"/>
-      <c r="R12" s="41"/>
+      <c r="R12" s="47"/>
       <c r="S12" s="41"/>
       <c r="T12" s="41"/>
       <c r="U12" s="41"/>
@@ -2099,7 +2108,7 @@
       <c r="O15" s="54"/>
       <c r="P15" s="54"/>
       <c r="Q15" s="54"/>
-      <c r="R15" s="45"/>
+      <c r="R15" s="54"/>
       <c r="S15" s="45"/>
       <c r="T15" s="45"/>
       <c r="U15" s="45"/>
@@ -2112,17 +2121,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2131,10 +2140,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2783,7 +2792,7 @@
         <v>84</v>
       </c>
       <c r="C48" s="8">
-        <v>4.1666666666666664E-2</v>
+        <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2791,78 +2800,102 @@
         <v>43986</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="8">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
+        <v>43986</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7">
+        <v>43986</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="8">
-        <v>4.1666666666666664E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="10" t="s">
+      <c r="C51" s="8">
+        <v>0.19097222222222221</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B52" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C50" s="11">
-        <f>SUM(C47:C49)</f>
-        <v>9.0277777777777762E-2</v>
-      </c>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="10"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="10"/>
-    </row>
-    <row r="52" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
-      <c r="C52" s="4"/>
+      <c r="C52" s="11">
+        <f>SUM(C47:C51)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="53" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="7"/>
-      <c r="C53" s="4"/>
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
       <c r="C54" s="4"/>
     </row>
-    <row r="55" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
-      <c r="B55" s="3"/>
       <c r="C55" s="4"/>
-      <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7"/>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="10"/>
+    <row r="57" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7"/>
       <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="7"/>
-      <c r="C59" s="4"/>
-    </row>
-    <row r="60" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="10"/>
+    </row>
+    <row r="60" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
-      <c r="B60" s="3"/>
       <c r="C60" s="4"/>
-      <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="10"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="10"/>
+      <c r="A61" s="7"/>
+      <c r="C61" s="4"/>
+    </row>
+    <row r="62" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="7"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="10"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout des derniers détails...Manque les derniers éléments dans la doc
</commit_message>
<xml_diff>
--- a/Documentation/Planning_TPI_Jauch.xlsx
+++ b/Documentation/Planning_TPI_Jauch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wal41\source\repos\LogoGo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0880AAD-05FA-429D-A02C-36972EB5644C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DD7F21-32ED-4BBB-AB11-192B62BCABE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
   <si>
     <t>Jour</t>
   </si>
@@ -322,21 +322,30 @@
   <si>
     <t>Avancement correct. Pas en retard mais le rythme pourrait être plus important au niveau de la doc.</t>
   </si>
+  <si>
+    <t>Rien à signaler</t>
+  </si>
+  <si>
+    <t>Total 5.juin</t>
+  </si>
+  <si>
+    <t>Corrections mineures et finalisation de certaines fonctionnalités</t>
+  </si>
+  <si>
+    <t>Ajout de MessageBoc lors de certaines situations, je me suis assurer que rien de puisse faire planter l'application.</t>
+  </si>
+  <si>
+    <t>Ajout des derniers thêmes…Manque planning effectif final en image</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -659,14 +668,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -688,145 +696,145 @@
     <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -868,8 +876,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D63" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D63" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:D55" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tâche" dataDxfId="2"/>
@@ -1192,450 +1200,450 @@
   <sheetData>
     <row r="2" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:26" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="55">
+      <c r="C3" s="54">
         <v>1</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="55">
+      <c r="D3" s="55"/>
+      <c r="E3" s="54">
         <v>2</v>
       </c>
-      <c r="F3" s="56"/>
-      <c r="G3" s="55">
+      <c r="F3" s="55"/>
+      <c r="G3" s="54">
         <v>3</v>
       </c>
-      <c r="H3" s="56"/>
-      <c r="I3" s="55">
+      <c r="H3" s="55"/>
+      <c r="I3" s="54">
         <v>4</v>
       </c>
-      <c r="J3" s="56"/>
-      <c r="K3" s="55">
+      <c r="J3" s="55"/>
+      <c r="K3" s="54">
         <v>5</v>
       </c>
-      <c r="L3" s="56"/>
-      <c r="M3" s="55">
+      <c r="L3" s="55"/>
+      <c r="M3" s="54">
         <v>6</v>
       </c>
-      <c r="N3" s="56"/>
-      <c r="O3" s="55">
+      <c r="N3" s="55"/>
+      <c r="O3" s="54">
         <v>7</v>
       </c>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="55">
+      <c r="P3" s="55"/>
+      <c r="Q3" s="54">
         <v>8</v>
       </c>
-      <c r="R3" s="56"/>
-      <c r="S3" s="55">
+      <c r="R3" s="55"/>
+      <c r="S3" s="54">
         <v>9</v>
       </c>
-      <c r="T3" s="56"/>
-      <c r="U3" s="55">
+      <c r="T3" s="55"/>
+      <c r="U3" s="54">
         <v>10</v>
       </c>
-      <c r="V3" s="56"/>
-      <c r="W3" s="55">
+      <c r="V3" s="55"/>
+      <c r="W3" s="54">
         <v>11</v>
       </c>
-      <c r="X3" s="56"/>
+      <c r="X3" s="55"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="2:26" ht="19.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="34">
         <v>1</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="35">
         <v>2</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="35">
         <v>3</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="35">
         <v>4</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>5</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="35">
         <v>6</v>
       </c>
-      <c r="I4" s="36">
+      <c r="I4" s="35">
         <v>7</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="35">
         <v>8</v>
       </c>
-      <c r="K4" s="36">
+      <c r="K4" s="35">
         <v>9</v>
       </c>
-      <c r="L4" s="36">
+      <c r="L4" s="35">
         <v>10</v>
       </c>
-      <c r="M4" s="36">
+      <c r="M4" s="35">
         <v>11</v>
       </c>
-      <c r="N4" s="36">
+      <c r="N4" s="35">
         <v>12</v>
       </c>
-      <c r="O4" s="36">
+      <c r="O4" s="35">
         <v>13</v>
       </c>
-      <c r="P4" s="36">
+      <c r="P4" s="35">
         <v>14</v>
       </c>
-      <c r="Q4" s="36">
+      <c r="Q4" s="35">
         <v>15</v>
       </c>
-      <c r="R4" s="36">
+      <c r="R4" s="35">
         <v>16</v>
       </c>
-      <c r="S4" s="36">
+      <c r="S4" s="35">
         <v>17</v>
       </c>
-      <c r="T4" s="36">
+      <c r="T4" s="35">
         <v>18</v>
       </c>
-      <c r="U4" s="36">
+      <c r="U4" s="35">
         <v>19</v>
       </c>
-      <c r="V4" s="36">
+      <c r="V4" s="35">
         <v>20</v>
       </c>
-      <c r="W4" s="36">
+      <c r="W4" s="35">
         <v>21</v>
       </c>
-      <c r="X4" s="37">
+      <c r="X4" s="36">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="2:26" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="24"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="23"/>
     </row>
     <row r="6" spans="2:26" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="26"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="25"/>
     </row>
     <row r="7" spans="2:26" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="26"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="25"/>
     </row>
     <row r="8" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="26"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="24"/>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="24"/>
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="25"/>
     </row>
     <row r="9" spans="2:26" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="26"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="25"/>
     </row>
     <row r="10" spans="2:26" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="26"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="25"/>
     </row>
     <row r="11" spans="2:26" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="26"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="25"/>
     </row>
     <row r="12" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
-      <c r="X12" s="26"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="25"/>
     </row>
     <row r="13" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="29"/>
-      <c r="R13" s="29"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
-      <c r="V13" s="29"/>
-      <c r="W13" s="29"/>
-      <c r="X13" s="26"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="25"/>
     </row>
     <row r="14" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="29"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="26"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="24"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="25"/>
     </row>
     <row r="15" spans="2:26" ht="31.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
-      <c r="W15" s="29"/>
-      <c r="X15" s="30"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="29"/>
     </row>
     <row r="16" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
-      <c r="R16" s="34"/>
-      <c r="S16" s="27"/>
-      <c r="T16" s="27"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="28"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="26"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="26"/>
+      <c r="V16" s="26"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="27"/>
     </row>
     <row r="17" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -1659,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:AB16"/>
+  <dimension ref="B1:X16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1671,454 +1679,452 @@
     <col min="3" max="24" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
+    <row r="1" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="54">
         <v>1</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="55">
+      <c r="D2" s="55"/>
+      <c r="E2" s="54">
         <v>2</v>
       </c>
-      <c r="F2" s="56"/>
-      <c r="G2" s="55">
+      <c r="F2" s="55"/>
+      <c r="G2" s="54">
         <v>3</v>
       </c>
-      <c r="H2" s="56"/>
-      <c r="I2" s="55">
+      <c r="H2" s="55"/>
+      <c r="I2" s="54">
         <v>4</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="55">
+      <c r="J2" s="55"/>
+      <c r="K2" s="54">
         <v>5</v>
       </c>
-      <c r="L2" s="56"/>
-      <c r="M2" s="55">
+      <c r="L2" s="55"/>
+      <c r="M2" s="54">
         <v>6</v>
       </c>
-      <c r="N2" s="56"/>
-      <c r="O2" s="55">
+      <c r="N2" s="55"/>
+      <c r="O2" s="54">
         <v>7</v>
       </c>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="55">
+      <c r="P2" s="55"/>
+      <c r="Q2" s="54">
         <v>8</v>
       </c>
-      <c r="R2" s="56"/>
-      <c r="S2" s="55">
+      <c r="R2" s="55"/>
+      <c r="S2" s="54">
         <v>9</v>
       </c>
-      <c r="T2" s="56"/>
-      <c r="U2" s="55">
+      <c r="T2" s="55"/>
+      <c r="U2" s="54">
         <v>10</v>
       </c>
-      <c r="V2" s="56"/>
-      <c r="W2" s="55">
+      <c r="V2" s="55"/>
+      <c r="W2" s="54">
         <v>11</v>
       </c>
-      <c r="X2" s="56"/>
-    </row>
-    <row r="3" spans="2:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="14" t="s">
+      <c r="X2" s="55"/>
+    </row>
+    <row r="3" spans="2:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="34">
         <v>1</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="35">
         <v>2</v>
       </c>
-      <c r="E3" s="36">
+      <c r="E3" s="35">
         <v>3</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="35">
         <v>4</v>
       </c>
-      <c r="G3" s="36">
+      <c r="G3" s="35">
         <v>5</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="35">
         <v>6</v>
       </c>
-      <c r="I3" s="36">
+      <c r="I3" s="35">
         <v>7</v>
       </c>
-      <c r="J3" s="36">
+      <c r="J3" s="35">
         <v>8</v>
       </c>
-      <c r="K3" s="36">
+      <c r="K3" s="35">
         <v>9</v>
       </c>
-      <c r="L3" s="36">
+      <c r="L3" s="35">
         <v>10</v>
       </c>
-      <c r="M3" s="36">
+      <c r="M3" s="35">
         <v>11</v>
       </c>
-      <c r="N3" s="36">
+      <c r="N3" s="35">
         <v>12</v>
       </c>
-      <c r="O3" s="36">
+      <c r="O3" s="35">
         <v>13</v>
       </c>
-      <c r="P3" s="36">
+      <c r="P3" s="35">
         <v>14</v>
       </c>
-      <c r="Q3" s="36">
+      <c r="Q3" s="35">
         <v>15</v>
       </c>
-      <c r="R3" s="36">
+      <c r="R3" s="35">
         <v>16</v>
       </c>
-      <c r="S3" s="36">
+      <c r="S3" s="35">
         <v>17</v>
       </c>
-      <c r="T3" s="36">
+      <c r="T3" s="35">
         <v>18</v>
       </c>
-      <c r="U3" s="36">
+      <c r="U3" s="35">
         <v>19</v>
       </c>
-      <c r="V3" s="36">
+      <c r="V3" s="35">
         <v>20</v>
       </c>
-      <c r="W3" s="36">
+      <c r="W3" s="35">
         <v>21</v>
       </c>
-      <c r="X3" s="37">
+      <c r="X3" s="36">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:28" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="2:24" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="39"/>
-    </row>
-    <row r="5" spans="2:28" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="14" t="s">
+      <c r="C4" s="50"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="38"/>
+    </row>
+    <row r="5" spans="2:24" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
-      <c r="Q5" s="41"/>
-      <c r="R5" s="41"/>
-      <c r="S5" s="41"/>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
-      <c r="V5" s="41"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="42"/>
-    </row>
-    <row r="6" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
+      <c r="C5" s="51"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+      <c r="X5" s="41"/>
+    </row>
+    <row r="6" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="42"/>
-    </row>
-    <row r="7" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="15" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+      <c r="X6" s="41"/>
+    </row>
+    <row r="7" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="41"/>
-      <c r="V7" s="41"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="42"/>
-    </row>
-    <row r="8" spans="2:28" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="14" t="s">
+      <c r="C7" s="42"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+      <c r="X7" s="41"/>
+    </row>
+    <row r="8" spans="2:24" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="41"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="41"/>
-      <c r="X8" s="42"/>
-    </row>
-    <row r="9" spans="2:28" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="15" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
+      <c r="V8" s="40"/>
+      <c r="W8" s="40"/>
+      <c r="X8" s="41"/>
+    </row>
+    <row r="9" spans="2:24" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="47"/>
-      <c r="O9" s="47"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="42"/>
-    </row>
-    <row r="10" spans="2:28" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
+      <c r="C9" s="42"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="41"/>
+    </row>
+    <row r="10" spans="2:24" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="47"/>
-      <c r="S10" s="41"/>
-      <c r="T10" s="41"/>
-      <c r="U10" s="41"/>
-      <c r="V10" s="41"/>
-      <c r="W10" s="41"/>
-      <c r="X10" s="42"/>
-    </row>
-    <row r="11" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
+      <c r="C10" s="42"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="40"/>
+      <c r="W10" s="40"/>
+      <c r="X10" s="41"/>
+    </row>
+    <row r="11" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="47"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="41"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="41"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="42"/>
-    </row>
-    <row r="12" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="14" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="46"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="40"/>
+      <c r="W11" s="40"/>
+      <c r="X11" s="41"/>
+    </row>
+    <row r="12" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="47"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
-      <c r="O12" s="47"/>
-      <c r="P12" s="47"/>
-      <c r="Q12" s="47"/>
-      <c r="R12" s="47"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="42"/>
-    </row>
-    <row r="13" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="14" t="s">
+      <c r="C12" s="51"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
+      <c r="P12" s="46"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="46"/>
+      <c r="S12" s="46"/>
+      <c r="T12" s="46"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="40"/>
+      <c r="W12" s="40"/>
+      <c r="X12" s="41"/>
+    </row>
+    <row r="13" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="42"/>
-    </row>
-    <row r="14" spans="2:28" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="15" t="s">
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+      <c r="X13" s="41"/>
+    </row>
+    <row r="14" spans="2:24" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="42"/>
-    </row>
-    <row r="15" spans="2:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="16" t="s">
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="40"/>
+      <c r="X14" s="41"/>
+    </row>
+    <row r="15" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="54"/>
-      <c r="O15" s="54"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="54"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="45"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="45"/>
-      <c r="W15" s="45"/>
-      <c r="X15" s="46"/>
-    </row>
-    <row r="16" spans="2:28" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="AB16" s="2"/>
-    </row>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="53"/>
+      <c r="R15" s="53"/>
+      <c r="S15" s="53"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
+      <c r="X15" s="45"/>
+    </row>
+    <row r="16" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="M2:N2"/>
@@ -2142,760 +2148,790 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="3"/>
+    <col min="1" max="1" width="12.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="6"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>43976</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>43976</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>43976</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>43976</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>6.25E-2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>43976</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>43976</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>43976</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>43976</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>43976</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>43976</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>6.25E-2</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:11" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <f>SUM(C2:C11)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>43977</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <v>1.3888888888888888E-2</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+      <c r="A15" s="6">
         <v>43977</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>43977</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>0.14583333333333334</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>43977</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
+      <c r="A18" s="6">
         <v>43977</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+    <row r="19" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <f>SUM(C13:C18)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>43978</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>43978</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="7">
         <v>0.11805555555555557</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>43978</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C22" s="7">
         <v>0.10416666666666667</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>43978</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>43978</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <f>SUM(C20:C24)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
+      <c r="A26" s="6">
         <v>43979</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C26" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
+    <row r="27" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
         <v>43979</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="8">
+      <c r="C27" s="7">
         <v>0.14583333333333334</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>43979</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="7">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>43979</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>43979</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <f>SUM(C26:C30)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
+      <c r="A32" s="6">
         <v>43980</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>43980</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <v>0.125</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
+      <c r="A34" s="6">
         <v>43980</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <v>0.125</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>43980</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="7">
         <v>7.2916666666666671E-2</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="10">
         <f>SUM(C32:C35)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7">
+      <c r="A37" s="6">
         <v>43984</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
+      <c r="A38" s="6">
         <v>43984</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="7">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7">
+    <row r="39" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6">
         <v>43984</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="7">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
         <v>43984</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C40" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7">
+    <row r="41" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
         <v>43984</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="7">
         <v>0.125</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="10">
         <f>SUM(C37:C41)</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7">
+      <c r="A43" s="6">
         <v>43985</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="8">
+      <c r="C43" s="7">
         <v>0.125</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7">
+      <c r="A44" s="6">
         <v>43985</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="7">
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
+      <c r="A45" s="6">
         <v>43985</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="8">
+      <c r="C45" s="7">
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C46" s="10">
         <f>SUM(C43:C45)</f>
         <v>0.33333333333333337</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7">
+      <c r="A47" s="6">
         <v>43986</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="7">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="7">
+      <c r="A48" s="6">
         <v>43986</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="7">
         <v>0.10416666666666667</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7">
+      <c r="A49" s="6">
         <v>43986</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49" s="7">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7">
+      <c r="A50" s="6">
         <v>43986</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="7">
         <v>1.0416666666666666E-2</v>
       </c>
+      <c r="D50" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7">
+      <c r="A51" s="6">
         <v>43986</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C51" s="8">
+      <c r="C51" s="7">
         <v>0.19097222222222221</v>
       </c>
     </row>
-    <row r="52" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="10" t="s">
+    <row r="52" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="10">
         <f>SUM(C47:C51)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="10"/>
+    <row r="53" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6">
+        <v>43987</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="7"/>
-      <c r="C54" s="4"/>
+      <c r="A54" s="6">
+        <v>43987</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="7">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="7"/>
-      <c r="C55" s="4"/>
+      <c r="A55" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="10">
+        <f>SUM(C53:C54)</f>
+        <v>0.33333333333333331</v>
+      </c>
     </row>
     <row r="56" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="7"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="3"/>
+      <c r="A56" s="6"/>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="7"/>
-      <c r="C58" s="4"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="10"/>
     </row>
     <row r="59" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="10"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="7"/>
-      <c r="C60" s="4"/>
+      <c r="A60" s="6"/>
+      <c r="C60" s="3"/>
     </row>
     <row r="61" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="7"/>
-      <c r="C61" s="4"/>
-    </row>
-    <row r="62" spans="1:4" s="10" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="7"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="3"/>
+      <c r="A61" s="6"/>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" s="9" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="6"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="10"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="10"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>